<commit_message>
Inserting data into a created table in a created SQLite database file
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weron\Desktop\projekty\Tkinter Data Entry Form Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977084E1-5547-43E6-A976-61A036AC7866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20EDA7B-2B99-498C-B71D-3A4F63FFDFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>First name</t>
   </si>
@@ -118,6 +118,60 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Marina</t>
+  </si>
+  <si>
+    <t>Osuna</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Domínguez</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Lucrecia</t>
+  </si>
+  <si>
+    <t>Hendrich</t>
+  </si>
+  <si>
+    <t>MSc.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Ander</t>
+  </si>
+  <si>
+    <t>Muñoz</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Guzmán</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -457,19 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
@@ -589,6 +643,145 @@
         <v>31</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>